<commit_message>
Quadros e gráficos atualizados
</commit_message>
<xml_diff>
--- a/downloads/quadros_forum_10M_2016_2017_2018_2019_2020_2021.xlsx
+++ b/downloads/quadros_forum_10M_2016_2017_2018_2019_2020_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrc/Library/CloudStorage/GoogleDrive-joaquim.carvalho@gmail.com/My Drive/CIPF-interno/Outputs/Dados CN-PLP/Fontes estatísticas/Exemplos/comtradeplus.un.org/api/downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6349B416-68AB-F247-BC1B-BA2EC1B499FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8CB3B2-9270-8045-8553-EB3AA84FAFD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="500" windowWidth="53260" windowHeight="31900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4340" yWindow="500" windowWidth="13060" windowHeight="21980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -126,9 +126,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -138,6 +135,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -452,848 +452,848 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.83203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+      <c r="A2" s="6">
         <v>2016</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>1564651.5704000001</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>168039.86240000001</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>1396611.7080000001</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="6"/>
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>6783120.0011</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>2197615.2765000002</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>4585504.7246000003</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>4875.4718999999996</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>4867.1437999999998</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>8.3280999999999992</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="6"/>
+      <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>78010.5337</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>14825.383099999999</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>63185.150600000001</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="6"/>
+      <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>2139.7687000000001</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>2123.6460000000002</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>16.122699999999998</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="6"/>
+      <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>178791.46679999999</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>130855.7797</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>47935.687100000003</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="6"/>
+      <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>558493.76139999996</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>400211.95260000002</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>158281.8088</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="6"/>
+      <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>642.22130000000004</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>640.44910000000004</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>1.7722</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-      <c r="B10" s="5" t="s">
+      <c r="A10" s="6"/>
+      <c r="B10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>16456.440600000002</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>16427.28</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>29.160599999999999</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+      <c r="A11" s="6">
         <v>2017</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>2295616.2692</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>225745.32250000001</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>2069870.9467</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="B12" s="5" t="s">
+      <c r="A12" s="6"/>
+      <c r="B12" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>8780769.3508000001</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>2895053.8234999999</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>5885715.5273000002</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
-      <c r="B13" s="5" t="s">
+      <c r="A13" s="6"/>
+      <c r="B13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>6924.7879999999996</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <v>6923.9870000000001</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <v>0.80100000000000005</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="B14" s="5" t="s">
+      <c r="A14" s="6"/>
+      <c r="B14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>165005.29819999999</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="3">
         <v>16621.795600000001</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <v>148383.50260000001</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
-      <c r="B15" s="5" t="s">
+      <c r="A15" s="6"/>
+      <c r="B15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>3412.6720999999998</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <v>3372.4346</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>40.237499999999997</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
-      <c r="B16" s="5" t="s">
+      <c r="A16" s="6"/>
+      <c r="B16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <v>183546.1354</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
         <v>130674.61350000001</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <v>52871.5219</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
-      <c r="B17" s="5" t="s">
+      <c r="A17" s="6"/>
+      <c r="B17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>558439.34680000006</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <v>344521.49440000003</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>213917.8524</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
-      <c r="B18" s="5" t="s">
+      <c r="A18" s="6"/>
+      <c r="B18" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <v>690.2568</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="3">
         <v>690.18579999999997</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="3">
         <v>7.0999999999999994E-2</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-      <c r="B19" s="5" t="s">
+      <c r="A19" s="6"/>
+      <c r="B19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="3">
         <v>13416.978999999999</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="3">
         <v>13259.662200000001</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="3">
         <v>157.3168</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
+      <c r="A20" s="6">
         <v>2018</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="3">
         <v>2807964.7461999999</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="3">
         <v>225313.7107</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="3">
         <v>2582651.0355000002</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
-      <c r="B21" s="5" t="s">
+      <c r="A21" s="6"/>
+      <c r="B21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="3">
         <v>11123463.917199999</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="3">
         <v>3366513.9186999998</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="3">
         <v>7756949.9984999998</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
-      <c r="B22" s="5" t="s">
+      <c r="A22" s="6"/>
+      <c r="B22" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="3">
         <v>7855.6148000000003</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="3">
         <v>7826.5751</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="3">
         <v>29.0397</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
-      <c r="B23" s="5" t="s">
+      <c r="A23" s="6"/>
+      <c r="B23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="3">
         <v>228451.84969999999</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="3">
         <v>14514.640100000001</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="3">
         <v>213937.2096</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="2"/>
-      <c r="B24" s="5" t="s">
+      <c r="A24" s="6"/>
+      <c r="B24" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="3">
         <v>3747.0387000000001</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="3">
         <v>2983.1705000000002</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="3">
         <v>763.8682</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="2"/>
-      <c r="B25" s="5" t="s">
+      <c r="A25" s="6"/>
+      <c r="B25" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="3">
         <v>249531.44779999999</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="3">
         <v>186178.09700000001</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="3">
         <v>63353.3508</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
-      <c r="B26" s="5" t="s">
+      <c r="A26" s="6"/>
+      <c r="B26" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="3">
         <v>599925.37280000001</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D26" s="3">
         <v>375019.81430000003</v>
       </c>
-      <c r="E26" s="4">
+      <c r="E26" s="3">
         <v>224905.55850000001</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="5" t="s">
+      <c r="A27" s="6"/>
+      <c r="B27" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="3">
         <v>730.43489999999997</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D27" s="3">
         <v>725.51239999999996</v>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="3">
         <v>4.9225000000000003</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="5" t="s">
+      <c r="A28" s="6"/>
+      <c r="B28" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="3">
         <v>13540.412</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="3">
         <v>13238.9717</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="3">
         <v>301.44029999999998</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
+      <c r="A29" s="6">
         <v>2019</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="3">
         <v>2589312.9558999999</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="3">
         <v>205572.74170000001</v>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="3">
         <v>2383740.2141999998</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
-      <c r="B30" s="5" t="s">
+      <c r="A30" s="6"/>
+      <c r="B30" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="3">
         <v>11550161.095899999</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="3">
         <v>3553906.3912</v>
       </c>
-      <c r="E30" s="4">
+      <c r="E30" s="3">
         <v>7996254.7046999997</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
-      <c r="B31" s="5" t="s">
+      <c r="A31" s="6"/>
+      <c r="B31" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31" s="3">
         <v>6419.5681999999997</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D31" s="3">
         <v>6416.6990999999998</v>
       </c>
-      <c r="E31" s="4">
+      <c r="E31" s="3">
         <v>2.8691</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
-      <c r="B32" s="5" t="s">
+      <c r="A32" s="6"/>
+      <c r="B32" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="3">
         <v>183626.85079999999</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D32" s="3">
         <v>11320.445100000001</v>
       </c>
-      <c r="E32" s="4">
+      <c r="E32" s="3">
         <v>172306.4057</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
-      <c r="B33" s="5" t="s">
+      <c r="A33" s="6"/>
+      <c r="B33" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="3">
         <v>4034.1037999999999</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D33" s="3">
         <v>3193.8678</v>
       </c>
-      <c r="E33" s="4">
+      <c r="E33" s="3">
         <v>840.23599999999999</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
-      <c r="B34" s="5" t="s">
+      <c r="A34" s="6"/>
+      <c r="B34" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="3">
         <v>267093.66440000001</v>
       </c>
-      <c r="D34" s="4">
+      <c r="D34" s="3">
         <v>195769.50409999999</v>
       </c>
-      <c r="E34" s="4">
+      <c r="E34" s="3">
         <v>71324.160300000003</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
-      <c r="B35" s="5" t="s">
+      <c r="A35" s="6"/>
+      <c r="B35" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35" s="3">
         <v>668875.28339999996</v>
       </c>
-      <c r="D35" s="4">
+      <c r="D35" s="3">
         <v>436643.82579999999</v>
       </c>
-      <c r="E35" s="4">
+      <c r="E35" s="3">
         <v>232231.45759999999</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
-      <c r="B36" s="5" t="s">
+      <c r="A36" s="6"/>
+      <c r="B36" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36" s="3">
         <v>893.42790000000002</v>
       </c>
-      <c r="D36" s="4">
+      <c r="D36" s="3">
         <v>892.05589999999995</v>
       </c>
-      <c r="E36" s="4">
+      <c r="E36" s="3">
         <v>1.3720000000000001</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="2"/>
-      <c r="B37" s="5" t="s">
+      <c r="A37" s="6"/>
+      <c r="B37" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C37" s="3">
         <v>16751.308700000001</v>
       </c>
-      <c r="D37" s="4">
+      <c r="D37" s="3">
         <v>14294.8758</v>
       </c>
-      <c r="E37" s="4">
+      <c r="E37" s="3">
         <v>2456.4328999999998</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="2">
+      <c r="A38" s="6">
         <v>2020</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38" s="3">
         <v>1650582.2542000001</v>
       </c>
-      <c r="D38" s="4">
+      <c r="D38" s="3">
         <v>174809.22039999999</v>
       </c>
-      <c r="E38" s="4">
+      <c r="E38" s="3">
         <v>1475773.0338000001</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="2"/>
-      <c r="B39" s="5" t="s">
+      <c r="A39" s="6"/>
+      <c r="B39" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C39" s="3">
         <v>12047043.6745</v>
       </c>
-      <c r="D39" s="4">
+      <c r="D39" s="3">
         <v>3495322.7524999999</v>
       </c>
-      <c r="E39" s="4">
+      <c r="E39" s="3">
         <v>8551720.9220000003</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="2"/>
-      <c r="B40" s="5" t="s">
+      <c r="A40" s="6"/>
+      <c r="B40" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C40" s="4">
+      <c r="C40" s="3">
         <v>7904.6670999999997</v>
       </c>
-      <c r="D40" s="4">
+      <c r="D40" s="3">
         <v>7783.6679000000004</v>
       </c>
-      <c r="E40" s="4">
+      <c r="E40" s="3">
         <v>120.9992</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="2"/>
-      <c r="B41" s="5" t="s">
+      <c r="A41" s="6"/>
+      <c r="B41" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C41" s="4">
+      <c r="C41" s="3">
         <v>130466.94409999999</v>
       </c>
-      <c r="D41" s="4">
+      <c r="D41" s="3">
         <v>12212.0216</v>
       </c>
-      <c r="E41" s="4">
+      <c r="E41" s="3">
         <v>118254.9225</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="2"/>
-      <c r="B42" s="5" t="s">
+      <c r="A42" s="6"/>
+      <c r="B42" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C42" s="4">
+      <c r="C42" s="3">
         <v>5143.6017000000002</v>
       </c>
-      <c r="D42" s="4">
+      <c r="D42" s="3">
         <v>5143.0636000000004</v>
       </c>
-      <c r="E42" s="4">
+      <c r="E42" s="3">
         <v>0.53810000000000002</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="2"/>
-      <c r="B43" s="5" t="s">
+      <c r="A43" s="6"/>
+      <c r="B43" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="4">
+      <c r="C43" s="3">
         <v>257956.71710000001</v>
       </c>
-      <c r="D43" s="4">
+      <c r="D43" s="3">
         <v>200006.85519999999</v>
       </c>
-      <c r="E43" s="4">
+      <c r="E43" s="3">
         <v>57949.861900000004</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="2"/>
-      <c r="B44" s="5" t="s">
+      <c r="A44" s="6"/>
+      <c r="B44" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C44" s="4">
+      <c r="C44" s="3">
         <v>695305.34169999999</v>
       </c>
-      <c r="D44" s="4">
+      <c r="D44" s="3">
         <v>418056.50679999997</v>
       </c>
-      <c r="E44" s="4">
+      <c r="E44" s="3">
         <v>277248.83490000002</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="2"/>
-      <c r="B45" s="5" t="s">
+      <c r="A45" s="6"/>
+      <c r="B45" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C45" s="4">
+      <c r="C45" s="3">
         <v>2036.0128</v>
       </c>
-      <c r="D45" s="4">
+      <c r="D45" s="3">
         <v>2031.3471999999999</v>
       </c>
-      <c r="E45" s="4">
+      <c r="E45" s="3">
         <v>4.6656000000000004</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="2"/>
-      <c r="B46" s="5" t="s">
+      <c r="A46" s="6"/>
+      <c r="B46" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C46" s="4">
+      <c r="C46" s="3">
         <v>19248.301200000002</v>
       </c>
-      <c r="D46" s="4">
+      <c r="D46" s="3">
         <v>19127.239699999998</v>
       </c>
-      <c r="E46" s="4">
+      <c r="E46" s="3">
         <v>121.0615</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="2">
+      <c r="A47" s="6">
         <v>2021</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C47" s="4">
+      <c r="C47" s="3">
         <v>2339977.6998000001</v>
       </c>
-      <c r="D47" s="4">
+      <c r="D47" s="3">
         <v>249154.5681</v>
       </c>
-      <c r="E47" s="4">
+      <c r="E47" s="3">
         <v>2090823.1317</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="2"/>
-      <c r="B48" s="5" t="s">
+      <c r="A48" s="6"/>
+      <c r="B48" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C48" s="4">
+      <c r="C48" s="3">
         <v>16349010.067399999</v>
       </c>
-      <c r="D48" s="4">
+      <c r="D48" s="3">
         <v>5361222.4392999997</v>
       </c>
-      <c r="E48" s="4">
+      <c r="E48" s="3">
         <v>10987787.6281</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="2"/>
-      <c r="B49" s="5" t="s">
+      <c r="A49" s="6"/>
+      <c r="B49" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C49" s="4">
+      <c r="C49" s="3">
         <v>8568.4660999999996</v>
       </c>
-      <c r="D49" s="4">
+      <c r="D49" s="3">
         <v>8453.7739000000001</v>
       </c>
-      <c r="E49" s="4">
+      <c r="E49" s="3">
         <v>114.6922</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="2"/>
-      <c r="B50" s="5" t="s">
+      <c r="A50" s="6"/>
+      <c r="B50" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C50" s="4">
+      <c r="C50" s="3">
         <v>133912.65590000001</v>
       </c>
-      <c r="D50" s="4">
+      <c r="D50" s="3">
         <v>12398.4094</v>
       </c>
-      <c r="E50" s="4">
+      <c r="E50" s="3">
         <v>121514.24649999999</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="2"/>
-      <c r="B51" s="5" t="s">
+      <c r="A51" s="6"/>
+      <c r="B51" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C51" s="4">
+      <c r="C51" s="3">
         <v>8888.0025000000005</v>
       </c>
-      <c r="D51" s="4">
+      <c r="D51" s="3">
         <v>8887.8914000000004</v>
       </c>
-      <c r="E51" s="4">
+      <c r="E51" s="3">
         <v>0.1111</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="2"/>
-      <c r="B52" s="5" t="s">
+      <c r="A52" s="6"/>
+      <c r="B52" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C52" s="4">
+      <c r="C52" s="3">
         <v>403673.23729999998</v>
       </c>
-      <c r="D52" s="4">
+      <c r="D52" s="3">
         <v>289560.5441</v>
       </c>
-      <c r="E52" s="4">
+      <c r="E52" s="3">
         <v>114112.69319999999</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="2"/>
-      <c r="B53" s="5" t="s">
+      <c r="A53" s="6"/>
+      <c r="B53" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C53" s="4">
+      <c r="C53" s="3">
         <v>880802.84629999998</v>
       </c>
-      <c r="D53" s="4">
+      <c r="D53" s="3">
         <v>535423.80830000003</v>
       </c>
-      <c r="E53" s="4">
+      <c r="E53" s="3">
         <v>345379.038</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" s="2"/>
-      <c r="B54" s="5" t="s">
+      <c r="A54" s="6"/>
+      <c r="B54" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C54" s="4">
+      <c r="C54" s="3">
         <v>1507.7311999999999</v>
       </c>
-      <c r="D54" s="4">
+      <c r="D54" s="3">
         <v>1494.4514999999999</v>
       </c>
-      <c r="E54" s="4">
+      <c r="E54" s="3">
         <v>13.2797</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" s="2"/>
-      <c r="B55" s="5" t="s">
+      <c r="A55" s="6"/>
+      <c r="B55" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C55" s="4">
+      <c r="C55" s="3">
         <v>37358.4568</v>
       </c>
-      <c r="D55" s="4">
+      <c r="D55" s="3">
         <v>26043.3279</v>
       </c>
-      <c r="E55" s="4">
+      <c r="E55" s="3">
         <v>11315.1289</v>
       </c>
     </row>

</xml_diff>